<commit_message>
Metric and Library Random
</commit_message>
<xml_diff>
--- a/SmashMOBA/Status Metric.xlsx
+++ b/SmashMOBA/Status Metric.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Black Box\Desktop\My Stuff\Unity\Game\Team_Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Black Box\Desktop\My Stuff\Unity\Peachy-Games\SmashMOBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Management Items" sheetId="5" r:id="rId1"/>
     <sheet name="Code Items" sheetId="1" r:id="rId2"/>
     <sheet name="Art Items" sheetId="3" r:id="rId3"/>
+    <sheet name="Version Tracker" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="102">
   <si>
     <t>World Collision</t>
   </si>
@@ -118,9 +119,6 @@
     <t>Still</t>
   </si>
   <si>
-    <t>Samurai</t>
-  </si>
-  <si>
     <t>Idle Right</t>
   </si>
   <si>
@@ -238,13 +236,103 @@
     <t>Jump Left</t>
   </si>
   <si>
-    <t>Saberman</t>
-  </si>
-  <si>
     <t>Loganman</t>
   </si>
   <si>
     <t>Determine naming convention (champs/heroes/etc.)</t>
+  </si>
+  <si>
+    <t>Hidekage</t>
+  </si>
+  <si>
+    <t>Layton</t>
+  </si>
+  <si>
+    <t>0.1.0</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Software Version</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Milestones</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
+  </si>
+  <si>
+    <t>0.3.0</t>
+  </si>
+  <si>
+    <t>0.4.0</t>
+  </si>
+  <si>
+    <t>0.5.0</t>
+  </si>
+  <si>
+    <t>Character and map integration</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>0.6.0</t>
+  </si>
+  <si>
+    <t>0.7.0</t>
+  </si>
+  <si>
+    <t>0.8.0</t>
+  </si>
+  <si>
+    <t>0.9.0</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Major update</t>
+  </si>
+  <si>
+    <t>Hitboxes developed</t>
+  </si>
+  <si>
+    <t>Builds</t>
+  </si>
+  <si>
+    <t>Networking code developed</t>
+  </si>
+  <si>
+    <t>20 characters developed</t>
+  </si>
+  <si>
+    <t>Steam release</t>
+  </si>
+  <si>
+    <t>Feature development/objectives</t>
+  </si>
+  <si>
+    <t>GUI developed</t>
   </si>
 </sst>
 </file>
@@ -274,7 +362,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,8 +375,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -673,12 +767,165 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -788,6 +1035,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -833,8 +1082,100 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1311,7 +1652,7 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -1599,7 +1940,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="57" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -1623,7 +1964,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
@@ -1645,7 +1986,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="16" t="s">
         <v>2</v>
       </c>
@@ -1667,7 +2008,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="17" t="s">
         <v>3</v>
       </c>
@@ -1689,7 +2030,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="17" t="s">
         <v>4</v>
       </c>
@@ -1711,7 +2052,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
@@ -1733,7 +2074,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="17" t="s">
         <v>5</v>
       </c>
@@ -1755,7 +2096,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="17" t="s">
         <v>7</v>
       </c>
@@ -1777,7 +2118,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
+      <c r="A11" s="58"/>
       <c r="B11" s="17" t="s">
         <v>8</v>
       </c>
@@ -1799,7 +2140,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="17" t="s">
         <v>9</v>
       </c>
@@ -1821,7 +2162,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="18" t="s">
         <v>10</v>
       </c>
@@ -1843,11 +2184,11 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="60" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -1867,9 +2208,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
+      <c r="A15" s="61"/>
       <c r="B15" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -1889,9 +2230,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
+      <c r="A16" s="61"/>
       <c r="B16" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -1911,9 +2252,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
+      <c r="A17" s="61"/>
       <c r="B17" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -1933,9 +2274,9 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
+      <c r="A18" s="61"/>
       <c r="B18" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
@@ -1955,9 +2296,9 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
+      <c r="A19" s="61"/>
       <c r="B19" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -1977,9 +2318,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
+      <c r="A20" s="61"/>
       <c r="B20" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -1999,9 +2340,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
+      <c r="A21" s="61"/>
       <c r="B21" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -2021,9 +2362,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
+      <c r="A22" s="61"/>
       <c r="B22" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -2043,9 +2384,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
+      <c r="A23" s="61"/>
       <c r="B23" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -2065,9 +2406,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
+      <c r="A24" s="61"/>
       <c r="B24" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -2087,9 +2428,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
+      <c r="A25" s="61"/>
       <c r="B25" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -2109,9 +2450,9 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
+      <c r="A26" s="61"/>
       <c r="B26" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -2131,9 +2472,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="59"/>
+      <c r="A27" s="61"/>
       <c r="B27" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
@@ -2153,9 +2494,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="59"/>
+      <c r="A28" s="61"/>
       <c r="B28" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -2175,9 +2516,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="59"/>
+      <c r="A29" s="61"/>
       <c r="B29" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -2197,9 +2538,9 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="59"/>
+      <c r="A30" s="61"/>
       <c r="B30" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
@@ -2219,9 +2560,9 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="59"/>
+      <c r="A31" s="61"/>
       <c r="B31" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
@@ -2241,9 +2582,9 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="59"/>
+      <c r="A32" s="61"/>
       <c r="B32" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" s="3">
         <v>0</v>
@@ -2263,9 +2604,9 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="59"/>
+      <c r="A33" s="61"/>
       <c r="B33" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" s="3">
         <v>0</v>
@@ -2285,9 +2626,9 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
+      <c r="A34" s="61"/>
       <c r="B34" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
@@ -2307,31 +2648,31 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="59"/>
+      <c r="A35" s="61"/>
       <c r="B35" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="8">
+        <f t="shared" ref="G35:G51" si="1">SUM(C35:F35)/4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="61"/>
+      <c r="B36" s="26" t="s">
         <v>47</v>
-      </c>
-      <c r="C35" s="3">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0</v>
-      </c>
-      <c r="E35" s="3">
-        <v>0</v>
-      </c>
-      <c r="F35" s="3">
-        <v>0</v>
-      </c>
-      <c r="G35" s="8">
-        <f t="shared" ref="G35:G66" si="1">SUM(C35:F35)/4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="59"/>
-      <c r="B36" s="26" t="s">
-        <v>48</v>
       </c>
       <c r="C36" s="3">
         <v>0</v>
@@ -2351,9 +2692,9 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="59"/>
+      <c r="A37" s="61"/>
       <c r="B37" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
@@ -2373,9 +2714,9 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="59"/>
+      <c r="A38" s="61"/>
       <c r="B38" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C38" s="3">
         <v>0</v>
@@ -2395,9 +2736,9 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="59"/>
+      <c r="A39" s="61"/>
       <c r="B39" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C39" s="3">
         <v>0</v>
@@ -2417,9 +2758,9 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="59"/>
+      <c r="A40" s="61"/>
       <c r="B40" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="3">
         <v>0</v>
@@ -2439,9 +2780,9 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="59"/>
+      <c r="A41" s="61"/>
       <c r="B41" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" s="3">
         <v>0</v>
@@ -2461,9 +2802,9 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="59"/>
+      <c r="A42" s="61"/>
       <c r="B42" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C42" s="3">
         <v>0</v>
@@ -2483,9 +2824,9 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="59"/>
+      <c r="A43" s="61"/>
       <c r="B43" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
@@ -2505,9 +2846,9 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="59"/>
+      <c r="A44" s="61"/>
       <c r="B44" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
@@ -2527,9 +2868,9 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="59"/>
+      <c r="A45" s="61"/>
       <c r="B45" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" s="3">
         <v>0</v>
@@ -2549,9 +2890,9 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="59"/>
+      <c r="A46" s="61"/>
       <c r="B46" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="3">
         <v>0</v>
@@ -2571,9 +2912,9 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="59"/>
+      <c r="A47" s="61"/>
       <c r="B47" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="3">
         <v>0</v>
@@ -2593,9 +2934,9 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="59"/>
+      <c r="A48" s="61"/>
       <c r="B48" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" s="3">
         <v>0</v>
@@ -2615,9 +2956,9 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="59"/>
+      <c r="A49" s="61"/>
       <c r="B49" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" s="3">
         <v>0</v>
@@ -2637,9 +2978,9 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="59"/>
+      <c r="A50" s="61"/>
       <c r="B50" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C50" s="3">
         <v>0</v>
@@ -2659,9 +3000,9 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="60"/>
+      <c r="A51" s="62"/>
       <c r="B51" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C51" s="10">
         <v>0</v>
@@ -2694,8 +3035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,11 +3071,11 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
-        <v>30</v>
+      <c r="A3" s="63" t="s">
+        <v>71</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="6">
         <v>0</v>
@@ -2754,7 +3095,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
@@ -2776,9 +3117,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="62"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -2798,9 +3139,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
+      <c r="A6" s="64"/>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -2820,9 +3161,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
-      <c r="B7" s="70" t="s">
-        <v>56</v>
+      <c r="A7" s="64"/>
+      <c r="B7" s="55" t="s">
+        <v>55</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -2842,9 +3183,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="70" t="s">
-        <v>54</v>
+      <c r="A8" s="64"/>
+      <c r="B8" s="55" t="s">
+        <v>53</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -2864,9 +3205,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
-      <c r="B9" s="70" t="s">
-        <v>55</v>
+      <c r="A9" s="64"/>
+      <c r="B9" s="55" t="s">
+        <v>54</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -2886,9 +3227,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
-      <c r="B10" s="70" t="s">
-        <v>33</v>
+      <c r="A10" s="64"/>
+      <c r="B10" s="55" t="s">
+        <v>32</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -2908,9 +3249,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
-      <c r="B11" s="70" t="s">
-        <v>34</v>
+      <c r="A11" s="64"/>
+      <c r="B11" s="55" t="s">
+        <v>33</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
@@ -2930,9 +3271,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -2952,9 +3293,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3">
         <v>0</v>
@@ -2974,9 +3315,9 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
@@ -2996,9 +3337,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
-      <c r="B15" s="70" t="s">
-        <v>68</v>
+      <c r="A15" s="64"/>
+      <c r="B15" s="55" t="s">
+        <v>67</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -3018,9 +3359,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="62"/>
-      <c r="B16" s="70" t="s">
-        <v>69</v>
+      <c r="A16" s="64"/>
+      <c r="B16" s="55" t="s">
+        <v>68</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -3040,9 +3381,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
@@ -3062,9 +3403,9 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
@@ -3084,9 +3425,9 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="62"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -3106,9 +3447,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
@@ -3128,9 +3469,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -3150,9 +3491,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="62"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -3172,9 +3513,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
@@ -3194,9 +3535,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="62"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -3216,9 +3557,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="62"/>
-      <c r="B25" s="70" t="s">
-        <v>46</v>
+      <c r="A25" s="64"/>
+      <c r="B25" s="55" t="s">
+        <v>45</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -3238,9 +3579,9 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
+      <c r="A26" s="64"/>
       <c r="B26" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -3260,9 +3601,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="62"/>
-      <c r="B27" s="70" t="s">
-        <v>48</v>
+      <c r="A27" s="64"/>
+      <c r="B27" s="55" t="s">
+        <v>47</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
@@ -3282,9 +3623,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="62"/>
-      <c r="B28" s="70" t="s">
-        <v>49</v>
+      <c r="A28" s="64"/>
+      <c r="B28" s="55" t="s">
+        <v>48</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -3304,9 +3645,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
-      <c r="B29" s="70" t="s">
-        <v>50</v>
+      <c r="A29" s="64"/>
+      <c r="B29" s="55" t="s">
+        <v>49</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -3326,9 +3667,9 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="3">
         <v>0</v>
@@ -3348,9 +3689,9 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
-      <c r="B31" s="70" t="s">
-        <v>52</v>
+      <c r="A31" s="64"/>
+      <c r="B31" s="55" t="s">
+        <v>51</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
@@ -3370,9 +3711,9 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" s="3">
         <v>0</v>
@@ -3392,9 +3733,9 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
-      <c r="B33" s="70" t="s">
-        <v>57</v>
+      <c r="A33" s="64"/>
+      <c r="B33" s="55" t="s">
+        <v>56</v>
       </c>
       <c r="C33" s="3">
         <v>0</v>
@@ -3414,9 +3755,9 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="62"/>
-      <c r="B34" s="70" t="s">
-        <v>58</v>
+      <c r="A34" s="64"/>
+      <c r="B34" s="55" t="s">
+        <v>57</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
@@ -3436,9 +3777,9 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="62"/>
-      <c r="B35" s="70" t="s">
-        <v>59</v>
+      <c r="A35" s="64"/>
+      <c r="B35" s="55" t="s">
+        <v>58</v>
       </c>
       <c r="C35" s="3">
         <v>0</v>
@@ -3458,9 +3799,9 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="62"/>
-      <c r="B36" s="70" t="s">
-        <v>60</v>
+      <c r="A36" s="64"/>
+      <c r="B36" s="55" t="s">
+        <v>59</v>
       </c>
       <c r="C36" s="3">
         <v>0</v>
@@ -3480,9 +3821,9 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="62"/>
-      <c r="B37" s="70" t="s">
-        <v>61</v>
+      <c r="A37" s="64"/>
+      <c r="B37" s="55" t="s">
+        <v>60</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
@@ -3502,9 +3843,9 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="62"/>
-      <c r="B38" s="70" t="s">
-        <v>62</v>
+      <c r="A38" s="64"/>
+      <c r="B38" s="55" t="s">
+        <v>61</v>
       </c>
       <c r="C38" s="3">
         <v>0</v>
@@ -3524,9 +3865,9 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="62"/>
-      <c r="B39" s="70" t="s">
-        <v>63</v>
+      <c r="A39" s="64"/>
+      <c r="B39" s="55" t="s">
+        <v>62</v>
       </c>
       <c r="C39" s="3">
         <v>0</v>
@@ -3546,9 +3887,9 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="62"/>
-      <c r="B40" s="70" t="s">
-        <v>64</v>
+      <c r="A40" s="64"/>
+      <c r="B40" s="55" t="s">
+        <v>63</v>
       </c>
       <c r="C40" s="3">
         <v>0</v>
@@ -3568,9 +3909,9 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="62"/>
-      <c r="B41" s="70" t="s">
-        <v>65</v>
+      <c r="A41" s="64"/>
+      <c r="B41" s="55" t="s">
+        <v>64</v>
       </c>
       <c r="C41" s="3">
         <v>0</v>
@@ -3590,9 +3931,9 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="63"/>
-      <c r="B42" s="71" t="s">
-        <v>66</v>
+      <c r="A42" s="65"/>
+      <c r="B42" s="56" t="s">
+        <v>65</v>
       </c>
       <c r="C42" s="10">
         <v>0</v>
@@ -3612,11 +3953,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="64" t="s">
-        <v>70</v>
+      <c r="A43" s="66" t="s">
+        <v>72</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C43" s="28">
         <v>0</v>
@@ -3636,7 +3977,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="65"/>
+      <c r="A44" s="67"/>
       <c r="B44" s="30" t="s">
         <v>29</v>
       </c>
@@ -3658,9 +3999,9 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="65"/>
+      <c r="A45" s="67"/>
       <c r="B45" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" s="31">
         <v>1</v>
@@ -3680,9 +4021,9 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="65"/>
+      <c r="A46" s="67"/>
       <c r="B46" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C46" s="31">
         <v>0</v>
@@ -3702,9 +4043,9 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="65"/>
+      <c r="A47" s="67"/>
       <c r="B47" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" s="31">
         <v>0</v>
@@ -3724,9 +4065,9 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="65"/>
+      <c r="A48" s="67"/>
       <c r="B48" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" s="31">
         <v>0</v>
@@ -3746,9 +4087,9 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="65"/>
+      <c r="A49" s="67"/>
       <c r="B49" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" s="31">
         <v>0</v>
@@ -3768,9 +4109,9 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="65"/>
+      <c r="A50" s="67"/>
       <c r="B50" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C50" s="31">
         <v>0</v>
@@ -3790,9 +4131,9 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="65"/>
+      <c r="A51" s="67"/>
       <c r="B51" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C51" s="31">
         <v>0</v>
@@ -3812,9 +4153,9 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="65"/>
+      <c r="A52" s="67"/>
       <c r="B52" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C52" s="31">
         <v>0</v>
@@ -3834,9 +4175,9 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="65"/>
+      <c r="A53" s="67"/>
       <c r="B53" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C53" s="31">
         <v>0</v>
@@ -3856,9 +4197,9 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="65"/>
+      <c r="A54" s="67"/>
       <c r="B54" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" s="31">
         <v>0</v>
@@ -3878,9 +4219,9 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="65"/>
+      <c r="A55" s="67"/>
       <c r="B55" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C55" s="31">
         <v>0</v>
@@ -3900,9 +4241,9 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="65"/>
+      <c r="A56" s="67"/>
       <c r="B56" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C56" s="31">
         <v>0</v>
@@ -3922,9 +4263,9 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="65"/>
+      <c r="A57" s="67"/>
       <c r="B57" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C57" s="31">
         <v>0</v>
@@ -3944,9 +4285,9 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="65"/>
+      <c r="A58" s="67"/>
       <c r="B58" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C58" s="31">
         <v>0</v>
@@ -3966,9 +4307,9 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="65"/>
+      <c r="A59" s="67"/>
       <c r="B59" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C59" s="31">
         <v>0</v>
@@ -3988,9 +4329,9 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="65"/>
+      <c r="A60" s="67"/>
       <c r="B60" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C60" s="31">
         <v>0</v>
@@ -4010,9 +4351,9 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="65"/>
+      <c r="A61" s="67"/>
       <c r="B61" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C61" s="31">
         <v>0</v>
@@ -4032,9 +4373,9 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="65"/>
+      <c r="A62" s="67"/>
       <c r="B62" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C62" s="31">
         <v>0</v>
@@ -4054,9 +4395,9 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="65"/>
+      <c r="A63" s="67"/>
       <c r="B63" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C63" s="31">
         <v>0</v>
@@ -4076,9 +4417,9 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="65"/>
+      <c r="A64" s="67"/>
       <c r="B64" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C64" s="31">
         <v>0</v>
@@ -4098,9 +4439,9 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="65"/>
+      <c r="A65" s="67"/>
       <c r="B65" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C65" s="31">
         <v>0</v>
@@ -4120,9 +4461,9 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="65"/>
+      <c r="A66" s="67"/>
       <c r="B66" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C66" s="31">
         <v>0</v>
@@ -4142,9 +4483,9 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="65"/>
+      <c r="A67" s="67"/>
       <c r="B67" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C67" s="31">
         <v>0</v>
@@ -4164,9 +4505,9 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="65"/>
+      <c r="A68" s="67"/>
       <c r="B68" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C68" s="31">
         <v>0</v>
@@ -4186,9 +4527,9 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="65"/>
+      <c r="A69" s="67"/>
       <c r="B69" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C69" s="31">
         <v>0</v>
@@ -4208,9 +4549,9 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="65"/>
+      <c r="A70" s="67"/>
       <c r="B70" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C70" s="31">
         <v>0</v>
@@ -4230,9 +4571,9 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="65"/>
+      <c r="A71" s="67"/>
       <c r="B71" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C71" s="31">
         <v>0</v>
@@ -4252,9 +4593,9 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="65"/>
+      <c r="A72" s="67"/>
       <c r="B72" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C72" s="31">
         <v>0</v>
@@ -4274,9 +4615,9 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="65"/>
+      <c r="A73" s="67"/>
       <c r="B73" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C73" s="31">
         <v>0</v>
@@ -4296,9 +4637,9 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="65"/>
+      <c r="A74" s="67"/>
       <c r="B74" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C74" s="31">
         <v>0</v>
@@ -4318,9 +4659,9 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="65"/>
+      <c r="A75" s="67"/>
       <c r="B75" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C75" s="31">
         <v>0</v>
@@ -4340,9 +4681,9 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="65"/>
+      <c r="A76" s="67"/>
       <c r="B76" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C76" s="31">
         <v>0</v>
@@ -4362,9 +4703,9 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="65"/>
+      <c r="A77" s="67"/>
       <c r="B77" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C77" s="31">
         <v>0</v>
@@ -4384,9 +4725,9 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="65"/>
+      <c r="A78" s="67"/>
       <c r="B78" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C78" s="31">
         <v>0</v>
@@ -4406,9 +4747,9 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="65"/>
+      <c r="A79" s="67"/>
       <c r="B79" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C79" s="31">
         <v>0</v>
@@ -4428,9 +4769,9 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="65"/>
+      <c r="A80" s="67"/>
       <c r="B80" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C80" s="31">
         <v>0</v>
@@ -4450,9 +4791,9 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="65"/>
+      <c r="A81" s="67"/>
       <c r="B81" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C81" s="31">
         <v>0</v>
@@ -4472,9 +4813,9 @@
       </c>
     </row>
     <row r="82" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="66"/>
+      <c r="A82" s="68"/>
       <c r="B82" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C82" s="34">
         <v>0</v>
@@ -4494,11 +4835,11 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="67" t="s">
-        <v>71</v>
+      <c r="A83" s="69" t="s">
+        <v>69</v>
       </c>
       <c r="B83" s="48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C83" s="49">
         <v>0</v>
@@ -4518,7 +4859,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="68"/>
+      <c r="A84" s="70"/>
       <c r="B84" s="4" t="s">
         <v>29</v>
       </c>
@@ -4540,9 +4881,9 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="68"/>
+      <c r="A85" s="70"/>
       <c r="B85" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C85" s="51">
         <v>1</v>
@@ -4562,9 +4903,9 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="68"/>
+      <c r="A86" s="70"/>
       <c r="B86" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C86" s="51">
         <v>0</v>
@@ -4584,9 +4925,9 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="68"/>
+      <c r="A87" s="70"/>
       <c r="B87" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C87" s="51">
         <v>0</v>
@@ -4606,9 +4947,9 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="68"/>
+      <c r="A88" s="70"/>
       <c r="B88" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C88" s="51">
         <v>0</v>
@@ -4628,9 +4969,9 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="68"/>
+      <c r="A89" s="70"/>
       <c r="B89" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C89" s="51">
         <v>0</v>
@@ -4650,9 +4991,9 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="68"/>
+      <c r="A90" s="70"/>
       <c r="B90" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C90" s="51">
         <v>0</v>
@@ -4672,9 +5013,9 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="68"/>
+      <c r="A91" s="70"/>
       <c r="B91" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C91" s="51">
         <v>0</v>
@@ -4694,9 +5035,9 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="68"/>
+      <c r="A92" s="70"/>
       <c r="B92" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C92" s="51">
         <v>0</v>
@@ -4716,9 +5057,9 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="68"/>
+      <c r="A93" s="70"/>
       <c r="B93" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C93" s="51">
         <v>0</v>
@@ -4738,9 +5079,9 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="68"/>
+      <c r="A94" s="70"/>
       <c r="B94" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C94" s="51">
         <v>0</v>
@@ -4760,9 +5101,9 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="68"/>
+      <c r="A95" s="70"/>
       <c r="B95" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C95" s="51">
         <v>0</v>
@@ -4782,9 +5123,9 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="68"/>
+      <c r="A96" s="70"/>
       <c r="B96" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C96" s="51">
         <v>0</v>
@@ -4804,9 +5145,9 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="68"/>
+      <c r="A97" s="70"/>
       <c r="B97" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C97" s="51">
         <v>0</v>
@@ -4826,9 +5167,9 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="68"/>
+      <c r="A98" s="70"/>
       <c r="B98" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C98" s="51">
         <v>0</v>
@@ -4848,9 +5189,9 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="68"/>
+      <c r="A99" s="70"/>
       <c r="B99" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C99" s="51">
         <v>0</v>
@@ -4865,14 +5206,14 @@
         <v>0</v>
       </c>
       <c r="G99" s="52">
-        <f t="shared" ref="G99:G130" si="3">SUM(C99:F99)/4</f>
+        <f t="shared" ref="G99:G122" si="3">SUM(C99:F99)/4</f>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="68"/>
+      <c r="A100" s="70"/>
       <c r="B100" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C100" s="51">
         <v>0</v>
@@ -4892,9 +5233,9 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="68"/>
+      <c r="A101" s="70"/>
       <c r="B101" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C101" s="51">
         <v>0</v>
@@ -4914,9 +5255,9 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="68"/>
+      <c r="A102" s="70"/>
       <c r="B102" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C102" s="51">
         <v>0</v>
@@ -4936,9 +5277,9 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="68"/>
+      <c r="A103" s="70"/>
       <c r="B103" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C103" s="51">
         <v>0</v>
@@ -4958,9 +5299,9 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="68"/>
+      <c r="A104" s="70"/>
       <c r="B104" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C104" s="51">
         <v>0</v>
@@ -4980,9 +5321,9 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="68"/>
+      <c r="A105" s="70"/>
       <c r="B105" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C105" s="51">
         <v>0</v>
@@ -5002,9 +5343,9 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="68"/>
+      <c r="A106" s="70"/>
       <c r="B106" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C106" s="51">
         <v>0</v>
@@ -5024,9 +5365,9 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="68"/>
+      <c r="A107" s="70"/>
       <c r="B107" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C107" s="51">
         <v>0</v>
@@ -5046,9 +5387,9 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="68"/>
+      <c r="A108" s="70"/>
       <c r="B108" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C108" s="51">
         <v>0</v>
@@ -5068,9 +5409,9 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="68"/>
+      <c r="A109" s="70"/>
       <c r="B109" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C109" s="51">
         <v>0</v>
@@ -5090,9 +5431,9 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="68"/>
+      <c r="A110" s="70"/>
       <c r="B110" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C110" s="51">
         <v>0</v>
@@ -5112,9 +5453,9 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="68"/>
+      <c r="A111" s="70"/>
       <c r="B111" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C111" s="51">
         <v>0</v>
@@ -5134,9 +5475,9 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="68"/>
+      <c r="A112" s="70"/>
       <c r="B112" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C112" s="51">
         <v>0</v>
@@ -5156,9 +5497,9 @@
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="68"/>
+      <c r="A113" s="70"/>
       <c r="B113" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C113" s="51">
         <v>0</v>
@@ -5178,9 +5519,9 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="68"/>
+      <c r="A114" s="70"/>
       <c r="B114" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C114" s="51">
         <v>0</v>
@@ -5200,9 +5541,9 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="68"/>
+      <c r="A115" s="70"/>
       <c r="B115" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C115" s="51">
         <v>0</v>
@@ -5222,9 +5563,9 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="68"/>
+      <c r="A116" s="70"/>
       <c r="B116" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C116" s="51">
         <v>0</v>
@@ -5244,9 +5585,9 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="68"/>
+      <c r="A117" s="70"/>
       <c r="B117" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C117" s="51">
         <v>0</v>
@@ -5266,9 +5607,9 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="68"/>
+      <c r="A118" s="70"/>
       <c r="B118" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C118" s="51">
         <v>0</v>
@@ -5288,9 +5629,9 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="68"/>
+      <c r="A119" s="70"/>
       <c r="B119" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C119" s="51">
         <v>0</v>
@@ -5310,9 +5651,9 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="68"/>
+      <c r="A120" s="70"/>
       <c r="B120" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C120" s="51">
         <v>0</v>
@@ -5332,9 +5673,9 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="68"/>
+      <c r="A121" s="70"/>
       <c r="B121" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C121" s="51">
         <v>0</v>
@@ -5354,9 +5695,9 @@
       </c>
     </row>
     <row r="122" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="69"/>
+      <c r="A122" s="71"/>
       <c r="B122" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C122" s="53">
         <v>0</v>
@@ -5384,4 +5725,2150 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L168"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.7109375" style="76" customWidth="1"/>
+    <col min="3" max="3" width="1.5703125" style="72" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2" style="72" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.5703125" style="72" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="78" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="75"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="77"/>
+    </row>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="99" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="101"/>
+      <c r="J2" s="96" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="97"/>
+      <c r="L2" s="98"/>
+    </row>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="89" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="84">
+        <v>0</v>
+      </c>
+      <c r="C4" s="85" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="85">
+        <v>1</v>
+      </c>
+      <c r="E4" s="85" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="86">
+        <v>0</v>
+      </c>
+      <c r="G4" s="102" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="93" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" s="94" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="95" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="80"/>
+      <c r="C5" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="79"/>
+      <c r="G5" s="103"/>
+      <c r="J5" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="90" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="80"/>
+      <c r="C6" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="79"/>
+      <c r="G6" s="103"/>
+      <c r="J6" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" s="90" t="s">
+        <v>79</v>
+      </c>
+      <c r="L6" s="41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="80"/>
+      <c r="C7" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="79"/>
+      <c r="G7" s="103"/>
+      <c r="J7" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="90" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="80"/>
+      <c r="C8" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="79"/>
+      <c r="G8" s="103"/>
+      <c r="J8" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="90" t="s">
+        <v>81</v>
+      </c>
+      <c r="L8" s="41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="80"/>
+      <c r="C9" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="79"/>
+      <c r="G9" s="103"/>
+      <c r="J9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" s="90" t="s">
+        <v>86</v>
+      </c>
+      <c r="L9" s="41"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="80"/>
+      <c r="C10" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="79"/>
+      <c r="G10" s="103"/>
+      <c r="J10" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10" s="90" t="s">
+        <v>87</v>
+      </c>
+      <c r="L10" s="41"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="80"/>
+      <c r="C11" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="79"/>
+      <c r="G11" s="103"/>
+      <c r="J11" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="90" t="s">
+        <v>88</v>
+      </c>
+      <c r="L11" s="41"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="80"/>
+      <c r="C12" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="79"/>
+      <c r="G12" s="103"/>
+      <c r="J12" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" s="90" t="s">
+        <v>89</v>
+      </c>
+      <c r="L12" s="41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="80"/>
+      <c r="C13" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="79"/>
+      <c r="G13" s="103"/>
+      <c r="J13" s="91" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="L13" s="43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="80"/>
+      <c r="C14" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="79"/>
+      <c r="G14" s="103"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="80"/>
+      <c r="C15" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="79"/>
+      <c r="G15" s="103"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="80"/>
+      <c r="C16" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="79"/>
+      <c r="G16" s="103"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="80"/>
+      <c r="C17" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="79"/>
+      <c r="G17" s="103"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="80"/>
+      <c r="C18" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="79"/>
+      <c r="G18" s="103"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="80"/>
+      <c r="C19" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="79"/>
+      <c r="G19" s="103"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="80"/>
+      <c r="C20" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="79"/>
+      <c r="G20" s="103"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="80"/>
+      <c r="C21" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="79"/>
+      <c r="G21" s="103"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="80"/>
+      <c r="C22" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="79"/>
+      <c r="G22" s="103"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="80"/>
+      <c r="C23" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="79"/>
+      <c r="G23" s="103"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="80"/>
+      <c r="C24" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="79"/>
+      <c r="G24" s="103"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="80"/>
+      <c r="C25" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="79"/>
+      <c r="G25" s="103"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="80"/>
+      <c r="C26" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="79"/>
+      <c r="G26" s="103"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="80"/>
+      <c r="C27" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="79"/>
+      <c r="G27" s="103"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="80"/>
+      <c r="C28" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="79"/>
+      <c r="G28" s="103"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="80"/>
+      <c r="C29" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="73"/>
+      <c r="E29" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="79"/>
+      <c r="G29" s="103"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="80"/>
+      <c r="C30" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="73"/>
+      <c r="E30" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="79"/>
+      <c r="G30" s="103"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="80"/>
+      <c r="C31" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="79"/>
+      <c r="G31" s="103"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="80"/>
+      <c r="C32" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="73"/>
+      <c r="E32" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="79"/>
+      <c r="G32" s="103"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="80"/>
+      <c r="C33" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="73"/>
+      <c r="E33" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="79"/>
+      <c r="G33" s="103"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="80"/>
+      <c r="C34" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="79"/>
+      <c r="G34" s="103"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="80"/>
+      <c r="C35" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="79"/>
+      <c r="G35" s="103"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="80"/>
+      <c r="C36" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="73"/>
+      <c r="E36" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" s="79"/>
+      <c r="G36" s="103"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="80"/>
+      <c r="C37" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="79"/>
+      <c r="G37" s="103"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="80"/>
+      <c r="C38" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F38" s="79"/>
+      <c r="G38" s="103"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="80"/>
+      <c r="C39" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" s="79"/>
+      <c r="G39" s="103"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="80"/>
+      <c r="C40" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="73"/>
+      <c r="E40" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" s="79"/>
+      <c r="G40" s="103"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="80"/>
+      <c r="C41" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F41" s="79"/>
+      <c r="G41" s="103"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="80"/>
+      <c r="C42" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" s="79"/>
+      <c r="G42" s="103"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="80"/>
+      <c r="C43" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="79"/>
+      <c r="G43" s="103"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="80"/>
+      <c r="C44" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="73"/>
+      <c r="E44" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F44" s="79"/>
+      <c r="G44" s="103"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="80"/>
+      <c r="C45" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="73"/>
+      <c r="E45" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F45" s="79"/>
+      <c r="G45" s="103"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="80"/>
+      <c r="C46" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F46" s="79"/>
+      <c r="G46" s="103"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="80"/>
+      <c r="C47" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="73"/>
+      <c r="E47" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" s="79"/>
+      <c r="G47" s="103"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="80"/>
+      <c r="C48" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="73"/>
+      <c r="E48" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F48" s="79"/>
+      <c r="G48" s="103"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="80"/>
+      <c r="C49" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" s="73"/>
+      <c r="E49" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F49" s="79"/>
+      <c r="G49" s="103"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="80"/>
+      <c r="C50" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="73"/>
+      <c r="E50" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" s="79"/>
+      <c r="G50" s="103"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="80"/>
+      <c r="C51" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" s="73"/>
+      <c r="E51" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" s="79"/>
+      <c r="G51" s="103"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="80"/>
+      <c r="C52" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" s="73"/>
+      <c r="E52" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F52" s="79"/>
+      <c r="G52" s="103"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="80"/>
+      <c r="C53" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" s="73"/>
+      <c r="E53" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="79"/>
+      <c r="G53" s="103"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="80"/>
+      <c r="C54" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54" s="73"/>
+      <c r="E54" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F54" s="79"/>
+      <c r="G54" s="103"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="80"/>
+      <c r="C55" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="73"/>
+      <c r="E55" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" s="79"/>
+      <c r="G55" s="104"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="80"/>
+      <c r="C56" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="73"/>
+      <c r="E56" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F56" s="79"/>
+      <c r="G56" s="104"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="80"/>
+      <c r="C57" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57" s="73"/>
+      <c r="E57" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F57" s="79"/>
+      <c r="G57" s="104"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="80"/>
+      <c r="C58" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F58" s="79"/>
+      <c r="G58" s="104"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="80"/>
+      <c r="C59" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" s="73"/>
+      <c r="E59" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F59" s="79"/>
+      <c r="G59" s="104"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="80"/>
+      <c r="C60" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60" s="73"/>
+      <c r="E60" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F60" s="79"/>
+      <c r="G60" s="104"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="80"/>
+      <c r="C61" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" s="73"/>
+      <c r="E61" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F61" s="79"/>
+      <c r="G61" s="104"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="80"/>
+      <c r="C62" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" s="73"/>
+      <c r="E62" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F62" s="79"/>
+      <c r="G62" s="104"/>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="80"/>
+      <c r="C63" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" s="73"/>
+      <c r="E63" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F63" s="79"/>
+      <c r="G63" s="104"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="80"/>
+      <c r="C64" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="73"/>
+      <c r="E64" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" s="79"/>
+      <c r="G64" s="104"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="80"/>
+      <c r="C65" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D65" s="73"/>
+      <c r="E65" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F65" s="79"/>
+      <c r="G65" s="104"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="80"/>
+      <c r="C66" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D66" s="73"/>
+      <c r="E66" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F66" s="79"/>
+      <c r="G66" s="104"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="80"/>
+      <c r="C67" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D67" s="73"/>
+      <c r="E67" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F67" s="79"/>
+      <c r="G67" s="104"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="80"/>
+      <c r="C68" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D68" s="73"/>
+      <c r="E68" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F68" s="79"/>
+      <c r="G68" s="104"/>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="80"/>
+      <c r="C69" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D69" s="73"/>
+      <c r="E69" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F69" s="79"/>
+      <c r="G69" s="104"/>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="80"/>
+      <c r="C70" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D70" s="73"/>
+      <c r="E70" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F70" s="79"/>
+      <c r="G70" s="104"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="80"/>
+      <c r="C71" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D71" s="73"/>
+      <c r="E71" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F71" s="79"/>
+      <c r="G71" s="104"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="80"/>
+      <c r="C72" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D72" s="73"/>
+      <c r="E72" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F72" s="79"/>
+      <c r="G72" s="104"/>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="80"/>
+      <c r="C73" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D73" s="73"/>
+      <c r="E73" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F73" s="79"/>
+      <c r="G73" s="104"/>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="80"/>
+      <c r="C74" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D74" s="73"/>
+      <c r="E74" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F74" s="79"/>
+      <c r="G74" s="104"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="80"/>
+      <c r="C75" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D75" s="73"/>
+      <c r="E75" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F75" s="79"/>
+      <c r="G75" s="104"/>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="80"/>
+      <c r="C76" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D76" s="73"/>
+      <c r="E76" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F76" s="79"/>
+      <c r="G76" s="104"/>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="80"/>
+      <c r="C77" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D77" s="73"/>
+      <c r="E77" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F77" s="79"/>
+      <c r="G77" s="104"/>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="80"/>
+      <c r="C78" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D78" s="73"/>
+      <c r="E78" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F78" s="79"/>
+      <c r="G78" s="104"/>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="80"/>
+      <c r="C79" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D79" s="73"/>
+      <c r="E79" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F79" s="79"/>
+      <c r="G79" s="104"/>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="80"/>
+      <c r="C80" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D80" s="73"/>
+      <c r="E80" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F80" s="79"/>
+      <c r="G80" s="104"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="80"/>
+      <c r="C81" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D81" s="73"/>
+      <c r="E81" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F81" s="79"/>
+      <c r="G81" s="104"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="80"/>
+      <c r="C82" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D82" s="73"/>
+      <c r="E82" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F82" s="79"/>
+      <c r="G82" s="104"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="80"/>
+      <c r="C83" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D83" s="73"/>
+      <c r="E83" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F83" s="79"/>
+      <c r="G83" s="104"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="80"/>
+      <c r="C84" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D84" s="73"/>
+      <c r="E84" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F84" s="79"/>
+      <c r="G84" s="104"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="80"/>
+      <c r="C85" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D85" s="73"/>
+      <c r="E85" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F85" s="79"/>
+      <c r="G85" s="104"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="80"/>
+      <c r="C86" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D86" s="73"/>
+      <c r="E86" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F86" s="79"/>
+      <c r="G86" s="104"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="80"/>
+      <c r="C87" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D87" s="73"/>
+      <c r="E87" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F87" s="79"/>
+      <c r="G87" s="104"/>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="80"/>
+      <c r="C88" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D88" s="73"/>
+      <c r="E88" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F88" s="79"/>
+      <c r="G88" s="104"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="80"/>
+      <c r="C89" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D89" s="73"/>
+      <c r="E89" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F89" s="79"/>
+      <c r="G89" s="104"/>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="80"/>
+      <c r="C90" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D90" s="73"/>
+      <c r="E90" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F90" s="79"/>
+      <c r="G90" s="104"/>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="80"/>
+      <c r="C91" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D91" s="73"/>
+      <c r="E91" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F91" s="79"/>
+      <c r="G91" s="104"/>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="80"/>
+      <c r="C92" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D92" s="73"/>
+      <c r="E92" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F92" s="79"/>
+      <c r="G92" s="104"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="80"/>
+      <c r="C93" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D93" s="73"/>
+      <c r="E93" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F93" s="79"/>
+      <c r="G93" s="104"/>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="80"/>
+      <c r="C94" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D94" s="73"/>
+      <c r="E94" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F94" s="79"/>
+      <c r="G94" s="104"/>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="80"/>
+      <c r="C95" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D95" s="73"/>
+      <c r="E95" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F95" s="79"/>
+      <c r="G95" s="104"/>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="80"/>
+      <c r="C96" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D96" s="73"/>
+      <c r="E96" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F96" s="79"/>
+      <c r="G96" s="104"/>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="80"/>
+      <c r="C97" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D97" s="73"/>
+      <c r="E97" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F97" s="79"/>
+      <c r="G97" s="104"/>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="80"/>
+      <c r="C98" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D98" s="73"/>
+      <c r="E98" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F98" s="79"/>
+      <c r="G98" s="104"/>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99" s="80"/>
+      <c r="C99" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D99" s="73"/>
+      <c r="E99" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F99" s="79"/>
+      <c r="G99" s="104"/>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="80"/>
+      <c r="C100" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D100" s="73"/>
+      <c r="E100" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F100" s="79"/>
+      <c r="G100" s="104"/>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101" s="80"/>
+      <c r="C101" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D101" s="73"/>
+      <c r="E101" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F101" s="79"/>
+      <c r="G101" s="104"/>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" s="80"/>
+      <c r="C102" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D102" s="73"/>
+      <c r="E102" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F102" s="79"/>
+      <c r="G102" s="104"/>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" s="80"/>
+      <c r="C103" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D103" s="73"/>
+      <c r="E103" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F103" s="79"/>
+      <c r="G103" s="104"/>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="80"/>
+      <c r="C104" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D104" s="73"/>
+      <c r="E104" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F104" s="79"/>
+      <c r="G104" s="104"/>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" s="80"/>
+      <c r="C105" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D105" s="73"/>
+      <c r="E105" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F105" s="79"/>
+      <c r="G105" s="104"/>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="80"/>
+      <c r="C106" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D106" s="73"/>
+      <c r="E106" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F106" s="79"/>
+      <c r="G106" s="104"/>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B107" s="80"/>
+      <c r="C107" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D107" s="73"/>
+      <c r="E107" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F107" s="79"/>
+      <c r="G107" s="104"/>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B108" s="80"/>
+      <c r="C108" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D108" s="73"/>
+      <c r="E108" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F108" s="79"/>
+      <c r="G108" s="104"/>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B109" s="80"/>
+      <c r="C109" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D109" s="73"/>
+      <c r="E109" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F109" s="79"/>
+      <c r="G109" s="104"/>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B110" s="80"/>
+      <c r="C110" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D110" s="73"/>
+      <c r="E110" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F110" s="79"/>
+      <c r="G110" s="104"/>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B111" s="80"/>
+      <c r="C111" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D111" s="73"/>
+      <c r="E111" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F111" s="79"/>
+      <c r="G111" s="104"/>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B112" s="80"/>
+      <c r="C112" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D112" s="73"/>
+      <c r="E112" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F112" s="79"/>
+      <c r="G112" s="104"/>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B113" s="80"/>
+      <c r="C113" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D113" s="73"/>
+      <c r="E113" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F113" s="79"/>
+      <c r="G113" s="104"/>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B114" s="80"/>
+      <c r="C114" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D114" s="73"/>
+      <c r="E114" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F114" s="79"/>
+      <c r="G114" s="104"/>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B115" s="80"/>
+      <c r="C115" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D115" s="73"/>
+      <c r="E115" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F115" s="79"/>
+      <c r="G115" s="104"/>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B116" s="80"/>
+      <c r="C116" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D116" s="73"/>
+      <c r="E116" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F116" s="79"/>
+      <c r="G116" s="104"/>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B117" s="80"/>
+      <c r="C117" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D117" s="73"/>
+      <c r="E117" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F117" s="79"/>
+      <c r="G117" s="104"/>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B118" s="80"/>
+      <c r="C118" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D118" s="73"/>
+      <c r="E118" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F118" s="79"/>
+      <c r="G118" s="104"/>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B119" s="80"/>
+      <c r="C119" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D119" s="73"/>
+      <c r="E119" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F119" s="79"/>
+      <c r="G119" s="104"/>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B120" s="80"/>
+      <c r="C120" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D120" s="73"/>
+      <c r="E120" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F120" s="79"/>
+      <c r="G120" s="104"/>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B121" s="80"/>
+      <c r="C121" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D121" s="73"/>
+      <c r="E121" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F121" s="79"/>
+      <c r="G121" s="104"/>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B122" s="80"/>
+      <c r="C122" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D122" s="73"/>
+      <c r="E122" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F122" s="79"/>
+      <c r="G122" s="104"/>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B123" s="80"/>
+      <c r="C123" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D123" s="73"/>
+      <c r="E123" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F123" s="79"/>
+      <c r="G123" s="104"/>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B124" s="80"/>
+      <c r="C124" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D124" s="73"/>
+      <c r="E124" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F124" s="79"/>
+      <c r="G124" s="104"/>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B125" s="80"/>
+      <c r="C125" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D125" s="73"/>
+      <c r="E125" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F125" s="79"/>
+      <c r="G125" s="104"/>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B126" s="80"/>
+      <c r="C126" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D126" s="73"/>
+      <c r="E126" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F126" s="79"/>
+      <c r="G126" s="104"/>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B127" s="80"/>
+      <c r="C127" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D127" s="73"/>
+      <c r="E127" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F127" s="79"/>
+      <c r="G127" s="104"/>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B128" s="80"/>
+      <c r="C128" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D128" s="73"/>
+      <c r="E128" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F128" s="79"/>
+      <c r="G128" s="104"/>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B129" s="80"/>
+      <c r="C129" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D129" s="73"/>
+      <c r="E129" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F129" s="79"/>
+      <c r="G129" s="104"/>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B130" s="80"/>
+      <c r="C130" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D130" s="73"/>
+      <c r="E130" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F130" s="79"/>
+      <c r="G130" s="104"/>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B131" s="80"/>
+      <c r="C131" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D131" s="73"/>
+      <c r="E131" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F131" s="79"/>
+      <c r="G131" s="104"/>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B132" s="80"/>
+      <c r="C132" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D132" s="73"/>
+      <c r="E132" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F132" s="79"/>
+      <c r="G132" s="104"/>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B133" s="80"/>
+      <c r="C133" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D133" s="73"/>
+      <c r="E133" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F133" s="79"/>
+      <c r="G133" s="104"/>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B134" s="80"/>
+      <c r="C134" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D134" s="73"/>
+      <c r="E134" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F134" s="79"/>
+      <c r="G134" s="104"/>
+    </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B135" s="80"/>
+      <c r="C135" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D135" s="73"/>
+      <c r="E135" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F135" s="79"/>
+      <c r="G135" s="104"/>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B136" s="80"/>
+      <c r="C136" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D136" s="73"/>
+      <c r="E136" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F136" s="79"/>
+      <c r="G136" s="104"/>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B137" s="80"/>
+      <c r="C137" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D137" s="73"/>
+      <c r="E137" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F137" s="79"/>
+      <c r="G137" s="104"/>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B138" s="80"/>
+      <c r="C138" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D138" s="73"/>
+      <c r="E138" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F138" s="79"/>
+      <c r="G138" s="104"/>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B139" s="80"/>
+      <c r="C139" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D139" s="73"/>
+      <c r="E139" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F139" s="79"/>
+      <c r="G139" s="104"/>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B140" s="80"/>
+      <c r="C140" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D140" s="73"/>
+      <c r="E140" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F140" s="79"/>
+      <c r="G140" s="104"/>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B141" s="80"/>
+      <c r="C141" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D141" s="73"/>
+      <c r="E141" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F141" s="79"/>
+      <c r="G141" s="104"/>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B142" s="80"/>
+      <c r="C142" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D142" s="73"/>
+      <c r="E142" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F142" s="79"/>
+      <c r="G142" s="104"/>
+    </row>
+    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B143" s="80"/>
+      <c r="C143" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D143" s="73"/>
+      <c r="E143" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F143" s="79"/>
+      <c r="G143" s="104"/>
+    </row>
+    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B144" s="80"/>
+      <c r="C144" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D144" s="73"/>
+      <c r="E144" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F144" s="79"/>
+      <c r="G144" s="104"/>
+    </row>
+    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B145" s="80"/>
+      <c r="C145" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D145" s="73"/>
+      <c r="E145" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F145" s="79"/>
+      <c r="G145" s="104"/>
+    </row>
+    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B146" s="80"/>
+      <c r="C146" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D146" s="73"/>
+      <c r="E146" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F146" s="79"/>
+      <c r="G146" s="104"/>
+    </row>
+    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B147" s="80"/>
+      <c r="C147" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D147" s="73"/>
+      <c r="E147" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F147" s="79"/>
+      <c r="G147" s="104"/>
+    </row>
+    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B148" s="80"/>
+      <c r="C148" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D148" s="73"/>
+      <c r="E148" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F148" s="79"/>
+      <c r="G148" s="104"/>
+    </row>
+    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B149" s="80"/>
+      <c r="C149" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D149" s="73"/>
+      <c r="E149" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F149" s="79"/>
+      <c r="G149" s="104"/>
+    </row>
+    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B150" s="80"/>
+      <c r="C150" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D150" s="73"/>
+      <c r="E150" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F150" s="79"/>
+      <c r="G150" s="104"/>
+    </row>
+    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B151" s="80"/>
+      <c r="C151" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D151" s="73"/>
+      <c r="E151" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F151" s="79"/>
+      <c r="G151" s="104"/>
+    </row>
+    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B152" s="80"/>
+      <c r="C152" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D152" s="73"/>
+      <c r="E152" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F152" s="79"/>
+      <c r="G152" s="104"/>
+    </row>
+    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B153" s="80"/>
+      <c r="C153" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D153" s="73"/>
+      <c r="E153" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F153" s="79"/>
+      <c r="G153" s="104"/>
+    </row>
+    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B154" s="80"/>
+      <c r="C154" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D154" s="73"/>
+      <c r="E154" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F154" s="79"/>
+      <c r="G154" s="104"/>
+    </row>
+    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B155" s="80"/>
+      <c r="C155" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D155" s="73"/>
+      <c r="E155" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F155" s="79"/>
+      <c r="G155" s="104"/>
+    </row>
+    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B156" s="80"/>
+      <c r="C156" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D156" s="73"/>
+      <c r="E156" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F156" s="79"/>
+      <c r="G156" s="104"/>
+    </row>
+    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B157" s="80"/>
+      <c r="C157" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D157" s="73"/>
+      <c r="E157" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F157" s="79"/>
+      <c r="G157" s="104"/>
+    </row>
+    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B158" s="80"/>
+      <c r="C158" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D158" s="73"/>
+      <c r="E158" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F158" s="79"/>
+      <c r="G158" s="104"/>
+    </row>
+    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B159" s="80"/>
+      <c r="C159" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D159" s="73"/>
+      <c r="E159" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F159" s="79"/>
+      <c r="G159" s="104"/>
+    </row>
+    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B160" s="80"/>
+      <c r="C160" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D160" s="73"/>
+      <c r="E160" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F160" s="79"/>
+      <c r="G160" s="104"/>
+    </row>
+    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B161" s="80"/>
+      <c r="C161" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D161" s="73"/>
+      <c r="E161" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F161" s="79"/>
+      <c r="G161" s="104"/>
+    </row>
+    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B162" s="80"/>
+      <c r="C162" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D162" s="73"/>
+      <c r="E162" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F162" s="79"/>
+      <c r="G162" s="104"/>
+    </row>
+    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B163" s="80"/>
+      <c r="C163" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D163" s="73"/>
+      <c r="E163" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F163" s="79"/>
+      <c r="G163" s="104"/>
+    </row>
+    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B164" s="80"/>
+      <c r="C164" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D164" s="73"/>
+      <c r="E164" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F164" s="79"/>
+      <c r="G164" s="104"/>
+    </row>
+    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B165" s="80"/>
+      <c r="C165" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D165" s="73"/>
+      <c r="E165" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F165" s="79"/>
+      <c r="G165" s="104"/>
+    </row>
+    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B166" s="80"/>
+      <c r="C166" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D166" s="73"/>
+      <c r="E166" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F166" s="79"/>
+      <c r="G166" s="104"/>
+    </row>
+    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B167" s="80"/>
+      <c r="C167" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D167" s="73"/>
+      <c r="E167" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="F167" s="79"/>
+      <c r="G167" s="104"/>
+    </row>
+    <row r="168" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B168" s="81"/>
+      <c r="C168" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="D168" s="82"/>
+      <c r="E168" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="F168" s="83"/>
+      <c r="G168" s="105"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>